<commit_message>
updated my time card
</commit_message>
<xml_diff>
--- a/Senior Design TimeCards.xlsx
+++ b/Senior Design TimeCards.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmad Alwakeel\Desktop\ahmed ee\tu-senior-design-hyperloop-computing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\HYPERLOOP\TU-Senior-Design-HyperLoop-Computing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sam" sheetId="1" r:id="rId1"/>
     <sheet name="Ahmed" sheetId="2" r:id="rId2"/>
     <sheet name="Travis" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
@@ -525,22 +525,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="A1:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5234375" customWidth="1"/>
-    <col min="2" max="2" width="16.41796875" customWidth="1"/>
-    <col min="4" max="4" width="25.89453125" customWidth="1"/>
-    <col min="5" max="5" width="20.3125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,37 +557,49 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+    <row r="2" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>42979.458333333336</v>
+      </c>
+      <c r="B2" s="2">
+        <v>42979.5</v>
+      </c>
       <c r="C2" s="3">
         <f>B2-A2</f>
-        <v>0</v>
+        <v>4.1666666664241347E-2</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+    <row r="3" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>42979.354166666664</v>
+      </c>
+      <c r="B3" s="4">
+        <v>42979.4375</v>
+      </c>
       <c r="C3" s="3">
         <f t="shared" ref="C3:C7" si="0">B3-A3</f>
-        <v>0</v>
+        <v>8.3333333335758653E-2</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+    <row r="4" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>42982.458333333336</v>
+      </c>
+      <c r="B4" s="4">
+        <v>42982.583333333336</v>
+      </c>
       <c r="C4" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3">
@@ -597,7 +609,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3">
@@ -607,7 +619,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="3">
@@ -617,14 +629,14 @@
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="8">
         <f>SUM(C2:C7)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -638,23 +650,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.3125" customWidth="1"/>
-    <col min="2" max="2" width="18.20703125" customWidth="1"/>
-    <col min="3" max="3" width="16.68359375" customWidth="1"/>
-    <col min="4" max="4" width="20.3125" customWidth="1"/>
-    <col min="5" max="5" width="35.68359375" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,7 +683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42979.416666666664</v>
       </c>
@@ -689,7 +701,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42979.854166666664</v>
       </c>
@@ -708,7 +720,7 @@
       </c>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -719,7 +731,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>42982.458333333336</v>
       </c>
@@ -737,7 +749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3">
@@ -747,7 +759,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3">
@@ -757,7 +769,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3">
@@ -767,7 +779,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="3">
@@ -777,7 +789,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="3">
@@ -787,7 +799,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
@@ -807,23 +819,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.41796875" customWidth="1"/>
-    <col min="2" max="2" width="15.20703125" customWidth="1"/>
-    <col min="3" max="3" width="14.41796875" customWidth="1"/>
-    <col min="4" max="5" width="15.20703125" customWidth="1"/>
-    <col min="6" max="6" width="52.20703125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="52.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,7 +855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42979.416666666664</v>
       </c>
@@ -862,7 +874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42979.354166666664</v>
       </c>
@@ -881,7 +893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
@@ -894,7 +906,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>42982.416666666664</v>
       </c>
@@ -913,7 +925,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="3"/>
@@ -921,7 +933,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
@@ -934,7 +946,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="5"/>
       <c r="E8" s="10"/>
     </row>

</xml_diff>

<commit_message>
worked design review ppt
</commit_message>
<xml_diff>
--- a/Senior Design TimeCards.xlsx
+++ b/Senior Design TimeCards.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Start Time</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Look at documentation sent from ORU and prepared for discussion in class</t>
+  </si>
+  <si>
+    <t>Rayzor Hall</t>
+  </si>
+  <si>
+    <t>Prepared Design Review #1 Presentation</t>
   </si>
 </sst>
 </file>
@@ -211,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -252,13 +258,16 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,10 +652,10 @@
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="8">
         <f>SUM(C2:C7)</f>
         <v>0.25</v>
@@ -813,10 +822,10 @@
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="8">
         <f>SUM(C5:C10)</f>
         <v>0.125</v>
@@ -833,10 +842,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,10 +916,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8">
         <f>SUM(C2:C3)</f>
         <v>8.333333334303461E-2</v>
@@ -958,10 +967,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16">
+      <c r="A7" s="14">
         <v>42985.666666666664</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <v>42985.708333333336</v>
       </c>
       <c r="C7" s="3">
@@ -977,21 +986,40 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="14">
+        <v>42986.625</v>
+      </c>
+      <c r="B8" s="14">
+        <v>42986.666666666664</v>
+      </c>
+      <c r="C8" s="3">
+        <f>B8-A8</f>
+        <v>4.1666666664241347E-2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="8">
+      <c r="B9" s="16"/>
+      <c r="C9" s="8">
         <f>SUM(C5:C6)</f>
         <v>0.25000000000727596</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="10"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
updated timecard up to week 2 hyperloop meeting
</commit_message>
<xml_diff>
--- a/Senior Design TimeCards.xlsx
+++ b/Senior Design TimeCards.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Google Drive\Senior Design 1\HyperLoop Computing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\HYPERLOOP\TU-Senior-Design-HyperLoop-Computing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sam" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Start Time</t>
   </si>
@@ -98,6 +98,24 @@
   </si>
   <si>
     <t>Meet with Hyperloop groups</t>
+  </si>
+  <si>
+    <t>discuss given requirements, formulate questions for the ORU team</t>
+  </si>
+  <si>
+    <t>debugged Ahmed's github, worked on requirements and workflow diagram</t>
+  </si>
+  <si>
+    <t>Rayzor Digital Lab</t>
+  </si>
+  <si>
+    <t>learned how to use GitHub, downloaded and installed, researched general workflow and branching</t>
+  </si>
+  <si>
+    <t>Reviewed documents provided by ORU, discussed conceptual diagram in relation to existing one</t>
+  </si>
+  <si>
+    <t>Met with entire hyperloop team, discussed checklist, scope, questions for ORU, and created an overall conceptual diagram</t>
   </si>
 </sst>
 </file>
@@ -220,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -270,6 +288,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,126 +578,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="105.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:5" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
+        <v>42979.416666666664</v>
+      </c>
+      <c r="B2" s="2">
         <v>42979.458333333336</v>
-      </c>
-      <c r="B2" s="2">
-        <v>42979.5</v>
       </c>
       <c r="C2" s="3">
         <f>B2-A2</f>
-        <v>4.1666666664241347E-2</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>42979.354166666664</v>
-      </c>
-      <c r="B3" s="4">
-        <v>42979.4375</v>
+        <v>4.1666666671517305E-2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>42979.854166666664</v>
+      </c>
+      <c r="B3" s="2">
+        <v>42979.9375</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C7" si="0">B3-A3</f>
+        <f t="shared" ref="C3" si="0">B3-A3</f>
         <v>8.3333333335758653E-2</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="8">
+        <f>SUM(C2:C3)</f>
+        <v>0.12500000000727596</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>42982.458333333336</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="2">
         <v>42982.583333333336</v>
       </c>
-      <c r="C4" s="3">
-        <f t="shared" si="0"/>
+      <c r="C5" s="3">
+        <f>B5-A5</f>
         <v>0.125</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>42986.583333333336</v>
+      </c>
+      <c r="B6" s="4">
+        <v>42986.614583333336</v>
+      </c>
       <c r="C6" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+        <f t="shared" ref="C6:C10" si="1">B6-A6</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>42988.75</v>
+      </c>
+      <c r="B7" s="4">
+        <v>42988.833333333336</v>
+      </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="8">
-        <f>SUM(C2:C7)</f>
-        <v>0.25</v>
+        <f t="shared" si="1"/>
+        <v>8.3333333335758653E-2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="8">
+        <f>SUM(C5:C10)</f>
+        <v>0.23958333333575865</v>
+      </c>
+      <c r="D11" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -679,19 +766,19 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42979.416666666664</v>
       </c>
@@ -726,7 +813,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42979.854166666664</v>
       </c>
@@ -745,7 +832,7 @@
       </c>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
@@ -756,7 +843,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>42982.458333333336</v>
       </c>
@@ -774,7 +861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3">
@@ -784,7 +871,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3">
@@ -794,7 +881,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3">
@@ -804,7 +891,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="3">
@@ -814,7 +901,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="3">
@@ -824,11 +911,11 @@
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="8">
         <f>SUM(C5:C10)</f>
         <v>0.125</v>
@@ -847,20 +934,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="52.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="52.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -880,7 +967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42979.416666666664</v>
       </c>
@@ -899,7 +986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42979.354166666664</v>
       </c>
@@ -918,11 +1005,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="8">
         <f>SUM(C2:C3)</f>
         <v>8.333333334303461E-2</v>
@@ -931,7 +1018,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>42982.416666666664</v>
       </c>
@@ -950,7 +1037,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>42983.625</v>
       </c>
@@ -969,7 +1056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>42985.666666666664</v>
       </c>
@@ -988,7 +1075,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>42986.625</v>
       </c>
@@ -1007,11 +1094,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="17"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="8">
         <f>SUM(C5:C6)</f>
         <v>0.25000000000727596</v>
@@ -1019,7 +1106,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>42988.75</v>
       </c>
@@ -1038,7 +1125,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="3">
@@ -1049,7 +1136,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="3">
@@ -1060,7 +1147,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="3">
@@ -1071,11 +1158,11 @@
       <c r="E13" s="10"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="17"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="8">
         <f>SUM(C10:C11)</f>
         <v>8.3333333335758653E-2</v>

</xml_diff>

<commit_message>
updated time card 9/15
</commit_message>
<xml_diff>
--- a/Senior Design TimeCards.xlsx
+++ b/Senior Design TimeCards.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>Start Time</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>researched UDOO processors, power consumption, created updated version of hardware conceptual diagram</t>
+  </si>
+  <si>
+    <t>Worked on project management budget</t>
+  </si>
+  <si>
+    <t>Researched possible propulsion ideas</t>
+  </si>
+  <si>
+    <t>Week 3 Total</t>
+  </si>
+  <si>
+    <t>Researched Linear Induction Motors for parameters based on criteria list</t>
   </si>
 </sst>
 </file>
@@ -158,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -237,11 +249,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -300,6 +366,50 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,7 +694,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,39 +843,44 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="A9" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36">
+        <f>SUM(C5:C8)</f>
+        <v>0.33333333333575865</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="A10" s="31">
+        <v>42992.875</v>
+      </c>
+      <c r="B10" s="31">
+        <v>42992.979166666664</v>
+      </c>
+      <c r="C10" s="32">
+        <f>B10-A10</f>
+        <v>0.10416666666424135</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="8">
-        <f>SUM(C5:C10)</f>
-        <v>0.33333333333575865</v>
-      </c>
-      <c r="D11" s="5"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -946,13 +1061,13 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="52.140625" customWidth="1"/>
@@ -1118,68 +1233,93 @@
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="30">
         <v>42988.75</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="30">
         <v>42988.833333333336</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="24">
         <f>B10-A10</f>
         <v>8.3333333335758653E-2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="23"/>
+      <c r="F10" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="3">
+      <c r="A11" s="30">
+        <v>42989.458333333336</v>
+      </c>
+      <c r="B11" s="30">
+        <v>42989.479166666664</v>
+      </c>
+      <c r="C11" s="24">
         <f>B11-A11</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="9"/>
+        <v>2.0833333328482695E-2</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="28" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="3">
+      <c r="A12" s="30">
+        <v>42989.625</v>
+      </c>
+      <c r="B12" s="30">
+        <v>42989.666666666664</v>
+      </c>
+      <c r="C12" s="24">
         <f>B12-A12</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
+        <v>4.1666666664241347E-2</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="3">
+      <c r="A13" s="30">
+        <v>42991.625</v>
+      </c>
+      <c r="B13" s="30">
+        <v>42991.666666666664</v>
+      </c>
+      <c r="C13" s="24">
         <f>B13-A13</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="15"/>
+        <v>4.1666666664241347E-2</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B14" s="20"/>
-      <c r="C14" s="8">
-        <f>SUM(C10:C11)</f>
-        <v>8.3333333335758653E-2</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="10"/>
+      <c r="C14" s="27">
+        <f>SUM(C10:C13)</f>
+        <v>0.18749999999272404</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
update time card 9/17
</commit_message>
<xml_diff>
--- a/Senior Design TimeCards.xlsx
+++ b/Senior Design TimeCards.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t>Start Time</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Researched Linear Induction Motors for parameters based on criteria list</t>
+  </si>
+  <si>
+    <t>Discussed wbs, budget, and propulsion research</t>
   </si>
 </sst>
 </file>
@@ -170,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -303,11 +306,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -361,12 +375,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -401,15 +409,27 @@
     <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="21" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,7 +816,7 @@
         <v>42986.614583333336</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" ref="C6:C10" si="1">B6-A6</f>
+        <f t="shared" ref="C6:C8" si="1">B6-A6</f>
         <v>3.125E-2</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -843,11 +863,11 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36">
+      <c r="B9" s="33"/>
+      <c r="C9" s="31">
         <f>SUM(C5:C8)</f>
         <v>0.33333333333575865</v>
       </c>
@@ -855,17 +875,17 @@
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31">
+      <c r="A10" s="29">
         <v>42992.875</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="29">
         <v>42992.979166666664</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="30">
         <f>B10-A10</f>
         <v>0.10416666666424135</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="19" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -873,14 +893,37 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="21"/>
+      <c r="A11" s="36">
+        <v>42995.75</v>
+      </c>
+      <c r="B11" s="36">
+        <v>42995.84375</v>
+      </c>
+      <c r="C11" s="37">
+        <f>B11-A11</f>
+        <v>9.375E-2</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="31">
+        <f>SUM(C10:C11)</f>
+        <v>0.19791666666424135</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -1038,10 +1081,10 @@
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="8">
         <f>SUM(C5:C10)</f>
         <v>0.125</v>
@@ -1132,10 +1175,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="8">
         <f>SUM(C2:C3)</f>
         <v>8.333333334303461E-2</v>
@@ -1221,10 +1264,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="8">
         <f>SUM(C5:C6)</f>
         <v>0.25000000000727596</v>
@@ -1233,93 +1276,93 @@
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="28">
         <v>42988.75</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="28">
         <v>42988.833333333336</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="22">
         <f>B10-A10</f>
         <v>8.3333333335758653E-2</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23" t="s">
+      <c r="E10" s="21"/>
+      <c r="F10" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="28">
         <v>42989.458333333336</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="28">
         <v>42989.479166666664</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="22">
         <f>B11-A11</f>
         <v>2.0833333328482695E-2</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="28" t="s">
+      <c r="E11" s="23"/>
+      <c r="F11" s="26" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="28">
         <v>42989.625</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="28">
         <v>42989.666666666664</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="22">
         <f>B12-A12</f>
         <v>4.1666666664241347E-2</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26" t="s">
+      <c r="E12" s="23"/>
+      <c r="F12" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="28">
         <v>42991.625</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="28">
         <v>42991.666666666664</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="22">
         <f>B13-A13</f>
         <v>4.1666666664241347E-2</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26" t="s">
+      <c r="E13" s="23"/>
+      <c r="F13" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="27">
+      <c r="B14" s="35"/>
+      <c r="C14" s="25">
         <f>SUM(C10:C13)</f>
         <v>0.18749999999272404</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Updated time card 9/20
</commit_message>
<xml_diff>
--- a/Senior Design TimeCards.xlsx
+++ b/Senior Design TimeCards.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t>Start Time</t>
   </si>
@@ -134,14 +134,21 @@
   </si>
   <si>
     <t>Discussed wbs, budget, and propulsion research</t>
+  </si>
+  <si>
+    <t>Case Athletic Center</t>
+  </si>
+  <si>
+    <t>Research Linear Induction Motors to correct cost, weight, efficiency criteria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="168" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -321,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -412,23 +419,32 @@
     <xf numFmtId="21" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -711,17 +727,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
     <col min="5" max="5" width="105.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -863,10 +879,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="33"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="31">
         <f>SUM(C5:C8)</f>
         <v>0.33333333333575865</v>
@@ -893,31 +909,49 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36">
+      <c r="A11" s="32">
         <v>42995.75</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B11" s="32">
         <v>42995.84375</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="33">
         <f>B11-A11</f>
         <v>9.375E-2</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="34" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="33"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="31">
         <f>SUM(C10:C11)</f>
         <v>0.19791666666424135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="39">
+        <v>42998.4375</v>
+      </c>
+      <c r="B13" s="40">
+        <v>42998.520833333336</v>
+      </c>
+      <c r="C13" s="41">
+        <f>B13-A13</f>
+        <v>8.3333333335758653E-2</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1081,10 +1115,10 @@
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="35"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="8">
         <f>SUM(C5:C10)</f>
         <v>0.125</v>
@@ -1175,10 +1209,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="8">
         <f>SUM(C2:C3)</f>
         <v>8.333333334303461E-2</v>
@@ -1264,10 +1298,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="8">
         <f>SUM(C5:C6)</f>
         <v>0.25000000000727596</v>
@@ -1352,10 +1386,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="35"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="25">
         <f>SUM(C10:C13)</f>
         <v>0.18749999999272404</v>

</xml_diff>